<commit_message>
my commit - 15082022
</commit_message>
<xml_diff>
--- a/Utilities/SuccessfulPatient_OpenMRS_DataFile.xlsx
+++ b/Utilities/SuccessfulPatient_OpenMRS_DataFile.xlsx
@@ -401,16 +401,16 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>iaojm</t>
+          <t>nqpxs</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>ahwdd</t>
+          <t>zimzm</t>
         </is>
       </c>
       <c r="C1" t="n">
-        <v>3795700153</v>
+        <v>8844065995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>